<commit_message>
Added Ticket to Ride: United Kingdom files
</commit_message>
<xml_diff>
--- a/Pennsylvania_Data_Files/Output/dependencies.xlsx
+++ b/Pennsylvania_Data_Files/Output/dependencies.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a684b2255d33441d/Data_science_projects/Ticket_To_Ride/Pennsylvania_Data_Files/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="67" documentId="6E115034D993DBB49C6F7F266440F07244894C87" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{CA72D93A-E189-44B3-BA09-A8C6D3566C50}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dependencies" sheetId="1" r:id="rId1"/>
@@ -138,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -972,14 +973,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>